<commit_message>
Updating spreadsheet with my part of the lab Also fixing small buildpath issue
</commit_message>
<xml_diff>
--- a/Artifacts/Documents/CS361 Chronotimer Test Plan Template.xlsx
+++ b/Artifacts/Documents/CS361 Chronotimer Test Plan Template.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rwmah\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{248FBC48-34FC-4F7C-9950-4981958A206B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16860" windowHeight="8415" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16860" windowHeight="8385" tabRatio="896"/>
   </bookViews>
   <sheets>
     <sheet name="Test Plan" sheetId="2" r:id="rId1"/>
@@ -20,7 +14,7 @@
     <sheet name="Test Cases Test Plan ID 4" sheetId="7" r:id="rId5"/>
     <sheet name="Test Cases Test Plan ID 5" sheetId="8" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -30,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="81">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -171,13 +165,115 @@
   </si>
   <si>
     <t>Fue</t>
+  </si>
+  <si>
+    <t>TC05.03</t>
+  </si>
+  <si>
+    <t>TC05.04</t>
+  </si>
+  <si>
+    <t>TC05.05</t>
+  </si>
+  <si>
+    <t>newrun while system on and current run exists</t>
+  </si>
+  <si>
+    <t>newrun with PARIND event type selected and no current run</t>
+  </si>
+  <si>
+    <t>newrun with GRP event type selected and no current run</t>
+  </si>
+  <si>
+    <t>TC05.06</t>
+  </si>
+  <si>
+    <t>TC05.07</t>
+  </si>
+  <si>
+    <t>newrun while system on and no current run and no run type specified</t>
+  </si>
+  <si>
+    <t>newrun with IND event type selected and no current run</t>
+  </si>
+  <si>
+    <t>newrun with PARGRP event type selected and no current run</t>
+  </si>
+  <si>
+    <t>newrun While System OFF</t>
+  </si>
+  <si>
+    <t>while power off - &lt;time&gt; newrun</t>
+  </si>
+  <si>
+    <t>currentRun == null</t>
+  </si>
+  <si>
+    <t>IllegalStateException</t>
+  </si>
+  <si>
+    <t>while power on and currentRun!=null - &lt;time&gt; newrun</t>
+  </si>
+  <si>
+    <t>currentRun == new Run</t>
+  </si>
+  <si>
+    <t>while power on and currentRun==null - &lt;time&gt; newrun</t>
+  </si>
+  <si>
+    <t>while power on, currentRun==null, and eventType="IND" - &lt;time&gt; newrun</t>
+  </si>
+  <si>
+    <t>currentRun == new IND()</t>
+  </si>
+  <si>
+    <t>while power on, currentRun==null, and eventType="PARIND" - &lt;time&gt; newrun</t>
+  </si>
+  <si>
+    <t>currentRun == new PARIND()</t>
+  </si>
+  <si>
+    <t>while power on, currentRun==null, and eventType="GRP" - &lt;time&gt; newrun</t>
+  </si>
+  <si>
+    <t>currentRun == new GRP()</t>
+  </si>
+  <si>
+    <t>while power on, currentRun==null, and eventType="PARGRP" - &lt;time&gt; newrun</t>
+  </si>
+  <si>
+    <t>currentRun == new PARGRP()</t>
+  </si>
+  <si>
+    <t>Time on 1 Computer</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>System off</t>
+  </si>
+  <si>
+    <t>newrun</t>
+  </si>
+  <si>
+    <t>power</t>
+  </si>
+  <si>
+    <t>event</t>
+  </si>
+  <si>
+    <t>1 Member of Team TBD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -632,25 +728,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B60"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="31.1875" customWidth="1"/>
+    <col min="2" max="2" width="31.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="6" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" s="6" customFormat="1" ht="57" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:2" s="7" customFormat="1">
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
@@ -658,7 +754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -666,12 +762,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -679,37 +775,37 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:2" s="7" customFormat="1">
       <c r="A14" s="7" t="s">
         <v>2</v>
       </c>
@@ -717,7 +813,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -725,12 +821,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -738,37 +834,37 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:2">
       <c r="A26" s="7" t="s">
         <v>2</v>
       </c>
@@ -776,7 +872,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -784,12 +880,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:2">
       <c r="A29">
         <v>3</v>
       </c>
@@ -797,37 +893,37 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:2">
       <c r="A38" s="7" t="s">
         <v>2</v>
       </c>
@@ -835,7 +931,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -843,12 +939,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:2">
       <c r="A41">
         <v>4</v>
       </c>
@@ -856,37 +952,37 @@
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:2">
       <c r="A43" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:2">
       <c r="A46" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:2">
       <c r="A47" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:2">
       <c r="A50" s="7" t="s">
         <v>2</v>
       </c>
@@ -894,7 +990,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:2">
       <c r="A51" t="s">
         <v>13</v>
       </c>
@@ -902,12 +998,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:2">
       <c r="A52" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:2">
       <c r="A53">
         <v>5</v>
       </c>
@@ -915,34 +1011,62 @@
         <v>41</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:2">
       <c r="A55" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="B55" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
       <c r="A56" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="B56" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
       <c r="A57" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="B57" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
       <c r="A58" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="B58" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
       <c r="A59" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="B59" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
       <c r="A60" t="s">
         <v>19</v>
+      </c>
+      <c r="B60" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="B61" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="B62" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -957,22 +1081,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="12.8125" customWidth="1"/>
-    <col min="2" max="2" width="21.8125" customWidth="1"/>
+    <col min="1" max="1" width="12.875" customWidth="1"/>
+    <col min="2" max="2" width="21.875" customWidth="1"/>
     <col min="3" max="3" width="37" customWidth="1"/>
-    <col min="4" max="4" width="15.1875" customWidth="1"/>
+    <col min="4" max="4" width="15.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="47.1" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -998,7 +1122,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1012,7 +1136,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1026,7 +1150,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -1040,7 +1164,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -1065,22 +1189,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="12.8125" customWidth="1"/>
-    <col min="2" max="2" width="21.8125" customWidth="1"/>
+    <col min="1" max="1" width="12.875" customWidth="1"/>
+    <col min="2" max="2" width="21.875" customWidth="1"/>
     <col min="3" max="3" width="37" customWidth="1"/>
-    <col min="4" max="4" width="15.1875" customWidth="1"/>
+    <col min="4" max="4" width="15.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="47.1" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1106,17 +1230,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:8">
       <c r="C5" s="3"/>
     </row>
   </sheetData>
@@ -1130,22 +1254,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADD78438-ADE5-46C7-B1C9-BBFECD99FEA4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="12.8125" customWidth="1"/>
-    <col min="2" max="2" width="21.8125" customWidth="1"/>
+    <col min="1" max="1" width="12.875" customWidth="1"/>
+    <col min="2" max="2" width="21.875" customWidth="1"/>
     <col min="3" max="3" width="37" customWidth="1"/>
-    <col min="4" max="4" width="15.1875" customWidth="1"/>
+    <col min="4" max="4" width="15.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="47.1" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1171,17 +1295,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:8">
       <c r="C5" s="3"/>
     </row>
   </sheetData>
@@ -1190,22 +1314,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60241042-81AD-4963-B965-AAC81A991AA6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="12.8125" customWidth="1"/>
-    <col min="2" max="2" width="21.8125" customWidth="1"/>
+    <col min="1" max="1" width="12.875" customWidth="1"/>
+    <col min="2" max="2" width="21.875" customWidth="1"/>
     <col min="3" max="3" width="37" customWidth="1"/>
-    <col min="4" max="4" width="15.1875" customWidth="1"/>
+    <col min="4" max="4" width="15.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="47.1" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1231,17 +1355,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:8">
       <c r="C5" s="3"/>
     </row>
   </sheetData>
@@ -1250,22 +1374,22 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB5B6B8B-C1CC-41D1-825A-41C774E013F2}">
-  <dimension ref="A1:H5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="12.8125" customWidth="1"/>
-    <col min="2" max="2" width="21.8125" customWidth="1"/>
-    <col min="3" max="3" width="37" customWidth="1"/>
-    <col min="4" max="4" width="15.1875" customWidth="1"/>
+    <col min="1" max="1" width="12.875" customWidth="1"/>
+    <col min="2" max="2" width="58.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="47.1" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1291,18 +1415,187 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="C5" s="3"/>
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" t="s">
+        <v>74</v>
+      </c>
+      <c r="H5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" t="s">
+        <v>74</v>
+      </c>
+      <c r="H6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" t="s">
+        <v>74</v>
+      </c>
+      <c r="H7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G8" t="s">
+        <v>74</v>
+      </c>
+      <c r="H8" t="s">
+        <v>74</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added my <TRIG> Test case to the Test Plan
</commit_message>
<xml_diff>
--- a/Artifacts/Documents/CS361 Chronotimer Test Plan Template.xlsx
+++ b/Artifacts/Documents/CS361 Chronotimer Test Plan Template.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19226"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{046A78E3-3DF5-4CD6-B05E-C798B06B6AA6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16860" windowHeight="8385" tabRatio="896"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16140" windowHeight="9615" tabRatio="896" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Plan" sheetId="2" r:id="rId1"/>
@@ -14,7 +15,8 @@
     <sheet name="Test Cases Test Plan ID 4" sheetId="7" r:id="rId5"/>
     <sheet name="Test Cases Test Plan ID 5" sheetId="8" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <oleSize ref="A1:C15"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="124">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -267,13 +269,154 @@
   </si>
   <si>
     <t>1 Member of Team TBD</t>
+  </si>
+  <si>
+    <t>&lt;TIME&gt; TRIG &lt;NUMBER&gt;</t>
+  </si>
+  <si>
+    <t>Trigger a channel (POWER state is OFF)</t>
+  </si>
+  <si>
+    <t>TC04.03</t>
+  </si>
+  <si>
+    <t>TC04.04</t>
+  </si>
+  <si>
+    <t>TC04.05</t>
+  </si>
+  <si>
+    <t>TC04.06</t>
+  </si>
+  <si>
+    <t>TC04.07</t>
+  </si>
+  <si>
+    <t>Execute method returns false and displays "power is off" message.</t>
+  </si>
+  <si>
+    <t>Execute method returns false and displays a "Need a RUN" message.</t>
+  </si>
+  <si>
+    <t>Execute method returns false and displays a "Need a Racer in RUN" message.</t>
+  </si>
+  <si>
+    <t>Trigger a channel (POWER state is ON, no channel number)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Execute method returns false and displays a "Need a Channel Number" message.
+</t>
+  </si>
+  <si>
+    <t>&lt;TIME&gt; TRIG</t>
+  </si>
+  <si>
+    <t>Trigger a channel (POWER state is ON, no RUN)</t>
+  </si>
+  <si>
+    <t>Trigger a channel (POWER state is ON, RUN created, no Racer)</t>
+  </si>
+  <si>
+    <t>&lt;TIME&gt; TRIG 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Execute method returns true and displays a "Racer &lt;bibNum&gt; started running" message.
+</t>
+  </si>
+  <si>
+    <t>&lt;TIME&gt; TRIG 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Execute method returns false and displays a "No Racer running" message.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trigger channel 2 (POWER state is ON, IND RUN created, Channel 1 inactive, Channel 2 active, 1 racer in queue)
+</t>
+  </si>
+  <si>
+    <t>Trigger channel 1 (POWER state is ON, IND RUN created, Channel 1 active, 1 racer in queue)</t>
+  </si>
+  <si>
+    <t>Trigger channel 1 (POWER state is ON, IND RUN created, Channel 1 inactive, 1 racer in queue)</t>
+  </si>
+  <si>
+    <t>TC04.08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trigger channel 2 (POWER state is ON, IND RUN created, Channel 1 active, Channel 2 active, 1 racer running)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Execute method returns true and displays a "Racer &lt;bibNum&gt; finished with a time of &lt;TIME&gt;" message.
+</t>
+  </si>
+  <si>
+    <t>&lt;TIME&gt; TRIG &lt;CHANNEL NUMBER&gt;</t>
+  </si>
+  <si>
+    <t>TC04.09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trigger any inactive channel (POWER state is ON, IND RUN created, &lt;CHANNEL NUMBER&gt; inactive)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Execute method returns false and displays a "Need to toggle channel 1 to active first" message.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Execute method returns false and displays a "Need to toggle the respective channel to active first" message.
+</t>
+  </si>
+  <si>
+    <t>JUNIT test, ChronoTimer class</t>
+  </si>
+  <si>
+    <t>TC04.10</t>
+  </si>
+  <si>
+    <t>Trigger channel 1 and 2 (POWER state is ON, PARIND RUN created, all channels are active, 1 racer in queue Lane 1, 1 racer in queue Lane 2)</t>
+  </si>
+  <si>
+    <t>&lt;TIME&gt; TRIG 1 and &lt;TIME&gt; TRIG 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Execute method returns true and displays a "Racer &lt;bibNum&gt; in Lane 1 started running" and after triggering channel 2, Execute method returns true and displays a "Racer &lt;bibNum&gt; in Lane 1 finshed with a time of &lt;TIME&gt;"  message.
+</t>
+  </si>
+  <si>
+    <t>TC04.11</t>
+  </si>
+  <si>
+    <t>Trigger channel 1 and 2 (POWER state is ON, PARIND RUN created, all channels are active, 1 racer finished in Lane 1, 1 racer in queue Lane 2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Execute method returns false and displays a "No queued racer in Lane 1" and after triggering channel 2, Execute method returns false and displays a "No racer running in Lane 1"  message.
+</t>
+  </si>
+  <si>
+    <t>TC04.12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Execute method returns true and displays a "Racer &lt;bibNum&gt; in Lane 2 started running" and after triggering channel 4, Execute method returns true and displays a "Racer &lt;bibNum&gt; in Lane 2 finshed with a time of &lt;TIME&gt;"  message.
+</t>
+  </si>
+  <si>
+    <t>Trigger channel 3 and 4 (POWER state is ON, PARIND RUN created, all channels are active, 1 racer finished in Lane 1, 1 racer in queue Lane 2)</t>
+  </si>
+  <si>
+    <t>TC04.13</t>
+  </si>
+  <si>
+    <t>Trigger channel 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -365,7 +508,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -384,6 +527,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -728,25 +875,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
     <col min="2" max="2" width="31.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="6" customFormat="1" ht="57" customHeight="1">
+    <row r="1" spans="1:2" s="6" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="7" customFormat="1">
+    <row r="2" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
@@ -754,7 +901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -762,12 +909,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>1</v>
       </c>
@@ -775,37 +922,37 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:2" s="7" customFormat="1">
+    <row r="14" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A14" s="7" t="s">
         <v>2</v>
       </c>
@@ -813,7 +960,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -821,12 +968,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A17">
         <v>2</v>
       </c>
@@ -834,37 +981,37 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A26" s="7" t="s">
         <v>2</v>
       </c>
@@ -872,7 +1019,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -880,12 +1027,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A29">
         <v>3</v>
       </c>
@@ -893,37 +1040,37 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A34" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A35" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A36" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A38" s="7" t="s">
         <v>2</v>
       </c>
@@ -931,7 +1078,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -939,12 +1086,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A40" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A41">
         <v>4</v>
       </c>
@@ -952,37 +1099,49 @@
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A43" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
+      <c r="B43" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A44" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="45" spans="1:2">
+      <c r="B44" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A45" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="46" spans="1:2">
+      <c r="B45" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A46" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="47" spans="1:2">
+      <c r="B46" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A47" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A48" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A50" s="7" t="s">
         <v>2</v>
       </c>
@@ -990,7 +1149,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A51" t="s">
         <v>13</v>
       </c>
@@ -998,12 +1157,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A52" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A53">
         <v>5</v>
       </c>
@@ -1011,7 +1170,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A55" t="s">
         <v>18</v>
       </c>
@@ -1019,7 +1178,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A56" t="s">
         <v>23</v>
       </c>
@@ -1027,7 +1186,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A57" t="s">
         <v>22</v>
       </c>
@@ -1035,7 +1194,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A58" t="s">
         <v>21</v>
       </c>
@@ -1043,7 +1202,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A59" t="s">
         <v>20</v>
       </c>
@@ -1051,7 +1210,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A60" t="s">
         <v>19</v>
       </c>
@@ -1059,12 +1218,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.5">
       <c r="B61" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.5">
       <c r="B62" t="s">
         <v>79</v>
       </c>
@@ -1081,14 +1240,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="12.875" customWidth="1"/>
     <col min="2" max="2" width="21.875" customWidth="1"/>
@@ -1096,7 +1255,7 @@
     <col min="4" max="4" width="15.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="47.1" customHeight="1">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="47.1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1122,7 +1281,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1136,7 +1295,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1150,7 +1309,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -1164,7 +1323,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -1189,14 +1348,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="12.875" customWidth="1"/>
     <col min="2" max="2" width="21.875" customWidth="1"/>
@@ -1204,7 +1363,7 @@
     <col min="4" max="4" width="15.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="47.1" customHeight="1">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="47.1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1230,17 +1389,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
       <c r="C5" s="3"/>
     </row>
   </sheetData>
@@ -1254,14 +1413,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="12.875" customWidth="1"/>
     <col min="2" max="2" width="21.875" customWidth="1"/>
@@ -1269,7 +1428,7 @@
     <col min="4" max="4" width="15.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="47.1" customHeight="1">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="47.1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1295,17 +1454,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
       <c r="C5" s="3"/>
     </row>
   </sheetData>
@@ -1314,22 +1473,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="12.875" customWidth="1"/>
-    <col min="2" max="2" width="21.875" customWidth="1"/>
+    <col min="2" max="2" width="138.1875" customWidth="1"/>
     <col min="3" max="3" width="37" customWidth="1"/>
-    <col min="4" max="4" width="15.25" customWidth="1"/>
+    <col min="4" max="4" width="64.9375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="47.1" customHeight="1">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="47.1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1355,18 +1514,325 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="B2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="C5" s="3"/>
+      <c r="B3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
+      <c r="A5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
+      <c r="A6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
+      <c r="A7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="E7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="E8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
+      <c r="A9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="G9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
+      <c r="A10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="78.75" x14ac:dyDescent="0.5">
+      <c r="A11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="63" x14ac:dyDescent="0.5">
+      <c r="A12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="78.75" x14ac:dyDescent="0.5">
+      <c r="A13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B13" t="s">
+        <v>121</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A14" t="s">
+        <v>122</v>
+      </c>
+      <c r="B14" t="s">
+        <v>123</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1374,14 +1840,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="12.875" customWidth="1"/>
     <col min="2" max="2" width="58.375" bestFit="1" customWidth="1"/>
@@ -1389,7 +1855,7 @@
     <col min="4" max="4" width="24.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="47.1" customHeight="1">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="47.1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1415,7 +1881,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -1441,7 +1907,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1467,7 +1933,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -1493,7 +1959,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -1519,7 +1985,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -1545,7 +2011,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>53</v>
       </c>
@@ -1571,7 +2037,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>54</v>
       </c>

</xml_diff>

<commit_message>
Update to test plan
</commit_message>
<xml_diff>
--- a/Artifacts/Documents/CS361 Chronotimer Test Plan Template.xlsx
+++ b/Artifacts/Documents/CS361 Chronotimer Test Plan Template.xlsx
@@ -3,7 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19226"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{046A78E3-3DF5-4CD6-B05E-C798B06B6AA6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\death\git\FastWatch361\Artifacts\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD7F9B9-2D77-4E24-83BC-18C88E7B004F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16140" windowHeight="9615" tabRatio="896" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,8 +20,7 @@
     <sheet name="Test Cases Test Plan ID 4" sheetId="7" r:id="rId5"/>
     <sheet name="Test Cases Test Plan ID 5" sheetId="8" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
-  <oleSize ref="A1:C15"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="144">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -409,7 +413,79 @@
     <t>TC04.13</t>
   </si>
   <si>
-    <t>Trigger channel 1</t>
+    <t>TC04.14</t>
+  </si>
+  <si>
+    <t>TC04.15</t>
+  </si>
+  <si>
+    <t>TC04.16</t>
+  </si>
+  <si>
+    <t>TC04.17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trigger channel 1 twice in GRP (POWER state is ON, GRP RUN created, all channels are active, bibNum 1, bibNum 2 and bibNum 3 racers in queue)
+</t>
+  </si>
+  <si>
+    <t>&lt;TIME&gt; TRIG 1 and &lt;TIME&gt; TRIG 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Execute method returns true and displays a "Group race has started" and after triggering channel 1 again, Execute method returns false and displays a "Group Race in progress"  message.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trigger channel 1 and channel 2 in GRP (POWER state is ON, GRP RUN created, all channels are active, bibNum 1, bibNum 2 and bibNum 3 racers in queue)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Execute method returns true and displays a "Group race has started" and after triggering channel 2, Execute method returns true and displays a "bibNum 1 finished in &lt;TIME&gt;"  message.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trigger any channels except 1 in PARGRP (POWER state is ON, PARGRP RUN created, all channels are active, bibNum 1, bibNum 2 and bibNum 3 racers in queue)
+</t>
+  </si>
+  <si>
+    <t>&lt;TIME&gt; TRIG &lt;CHANNEL NUMBER except 1&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Execute method returns false and displays a "Channel not supported"  message.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trigger channel 1 in PARGRP (POWER state is ON, PARGRP RUN created, all channels are active, bibNum 1, bibNum 2 and bibNum 3 racers in queue)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Execute method returns true and displays a "Parallel Group race has started" message.
+</t>
+  </si>
+  <si>
+    <t>&lt;TIME&gt; TRIG 3 and &lt;TIME&gt; TRIG 4</t>
+  </si>
+  <si>
+    <t>&lt;TIME&gt; TRIG 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trigger channel 3 in PARGRP (POWER state is ON, PARGRP RUN created, all channels are active, bibNum 1, bibNum 2 and bibNum 3 racers are running)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Execute method returns true and displays a "bibNum 3 has finished in &lt;TIME&gt;" message.
+</t>
+  </si>
+  <si>
+    <t>TC04.18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trigger channel 3 in PARGRP (POWER state is ON, PARGRP RUN created, all channels are active, bibNum 1, bibNum 2 are running and bibNum 3 is finished)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Execute method returns false and displays a "No racer is in Lane 3"  message.
+</t>
   </si>
 </sst>
 </file>
@@ -1474,10 +1550,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -1808,7 +1884,7 @@
         <v>121</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>114</v>
+        <v>137</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>120</v>
@@ -1826,13 +1902,164 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:8" ht="63" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>122</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="63" x14ac:dyDescent="0.5">
+      <c r="A15" t="s">
         <v>123</v>
       </c>
+      <c r="B15" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
+      <c r="A16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
+      <c r="A17" t="s">
+        <v>125</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
+      <c r="A18" t="s">
+        <v>126</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A19" t="s">
+        <v>141</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="B20" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
excel spreadheet - riley
</commit_message>
<xml_diff>
--- a/Artifacts/Documents/CS361 Chronotimer Test Plan Template.xlsx
+++ b/Artifacts/Documents/CS361 Chronotimer Test Plan Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\death\git\FastWatch361\Artifacts\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rwmah\Documents\CS361\FastWatch\Artifacts\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD7F9B9-2D77-4E24-83BC-18C88E7B004F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9EBE84D-80E5-440C-AC00-9352B53EC9EA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16140" windowHeight="9615" tabRatio="896" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16140" windowHeight="9615" tabRatio="896" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Plan" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="160">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -486,6 +486,54 @@
   <si>
     <t xml:space="preserve">Execute method returns false and displays a "No racer is in Lane 3"  message.
 </t>
+  </si>
+  <si>
+    <t>JUNIT test</t>
+  </si>
+  <si>
+    <t>&lt;TIME&gt; CONN &lt;NUMBER&gt; &lt;TYPE&gt;</t>
+  </si>
+  <si>
+    <t>Fail to connect as power is off</t>
+  </si>
+  <si>
+    <t>Power Off Connection</t>
+  </si>
+  <si>
+    <t>Sensor &lt;number&gt; is connected</t>
+  </si>
+  <si>
+    <t>Connection while connected</t>
+  </si>
+  <si>
+    <t>Sensor &lt;number&gt; is already connected</t>
+  </si>
+  <si>
+    <t>TC03.03</t>
+  </si>
+  <si>
+    <t>Disconnect while connected</t>
+  </si>
+  <si>
+    <t>Sensor &lt;number&gt; is disconnected</t>
+  </si>
+  <si>
+    <t>Power On Connection/ Connection while disconnected</t>
+  </si>
+  <si>
+    <t>TC03.05</t>
+  </si>
+  <si>
+    <t>TC03.04</t>
+  </si>
+  <si>
+    <t>Disconnect while Disconnected</t>
+  </si>
+  <si>
+    <t>TC03.06</t>
+  </si>
+  <si>
+    <t>Power Off Disconnect</t>
   </si>
 </sst>
 </file>
@@ -954,8 +1002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B62"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -1119,6 +1167,9 @@
     <row r="31" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
         <v>18</v>
+      </c>
+      <c r="B31" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.5">
@@ -1428,7 +1479,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H3"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -1490,18 +1541,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="12.875" customWidth="1"/>
-    <col min="2" max="2" width="21.875" customWidth="1"/>
+    <col min="2" max="2" width="48.5625" customWidth="1"/>
     <col min="3" max="3" width="37" customWidth="1"/>
-    <col min="4" max="4" width="15.25" customWidth="1"/>
+    <col min="4" max="4" width="35.4375" customWidth="1"/>
+    <col min="5" max="5" width="34.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="47.1" customHeight="1" x14ac:dyDescent="0.5">
@@ -1534,14 +1586,160 @@
       <c r="A2" t="s">
         <v>31</v>
       </c>
+      <c r="B2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>32</v>
       </c>
+      <c r="B3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D4" t="s">
+        <v>150</v>
+      </c>
+      <c r="E4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="C5" s="3"/>
+      <c r="A5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B6" t="s">
+        <v>157</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A7" t="s">
+        <v>158</v>
+      </c>
+      <c r="B7" t="s">
+        <v>159</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="C8" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1552,8 +1750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>

</xml_diff>